<commit_message>
Codigo que aplica el calculo de la tension requerida
Este es el sketch tentativo de el sistema de potencia con la libreria
del bioimpedanciometro incluida
</commit_message>
<xml_diff>
--- a/Bioimpedanciometro_Sketch_Funcional_2.0/Datos Bioimpedanciometro.xlsx
+++ b/Bioimpedanciometro_Sketch_Funcional_2.0/Datos Bioimpedanciometro.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$E$5:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja2!$E$5:$F$11</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>Valor medido</t>
   </si>
@@ -96,6 +97,48 @@
   <si>
     <t>Valor</t>
   </si>
+  <si>
+    <t>SENSADO DE TEJIDO BIOIMPEDANCIOMETRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ER-Piel (Placa Completa)[Ω]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ER-Piel (Media Placa)[Ω]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ER-Piel (Placa Espalda)[Ω]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ER-Piel (1/4 Placa)[Ω]</t>
+  </si>
+  <si>
+    <t>*Cambio de Extremidad</t>
+  </si>
+  <si>
+    <t>Impedancia Carne [Ω]</t>
+  </si>
+  <si>
+    <t>Impedancia Infinita [Ω]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impedancia Carne con 5V [Ω] </t>
+  </si>
+  <si>
+    <t>Valor Maximo</t>
+  </si>
+  <si>
+    <t>Valor Minimo</t>
+  </si>
+  <si>
+    <t>Valor Limite Deteccion de Placa</t>
+  </si>
+  <si>
+    <t>Valor Limite Deteccion de Bio</t>
+  </si>
+  <si>
+    <t>Valor desde la espalda a la mano</t>
+  </si>
 </sst>
 </file>
 
@@ -131,15 +174,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -186,11 +253,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,12 +338,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,11 +600,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="86940976"/>
-        <c:axId val="86942608"/>
+        <c:axId val="-1456634416"/>
+        <c:axId val="-1456633872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86940976"/>
+        <c:axId val="-1456634416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,7 +647,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86942608"/>
+        <c:crossAx val="-1456633872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -509,7 +655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86942608"/>
+        <c:axId val="-1456633872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -560,7 +706,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86940976"/>
+        <c:crossAx val="-1456634416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -836,11 +982,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="404658976"/>
-        <c:axId val="404670944"/>
+        <c:axId val="-1456637680"/>
+        <c:axId val="-1456637136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="404658976"/>
+        <c:axId val="-1456637680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +1029,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404670944"/>
+        <c:crossAx val="-1456637136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -891,7 +1037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="404670944"/>
+        <c:axId val="-1456637136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,7 +1088,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404658976"/>
+        <c:crossAx val="-1456637680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1226,11 +1372,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404661696"/>
-        <c:axId val="404658432"/>
+        <c:axId val="-1456633328"/>
+        <c:axId val="-1456636592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404661696"/>
+        <c:axId val="-1456633328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,12 +1428,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404658432"/>
+        <c:crossAx val="-1456636592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404658432"/>
+        <c:axId val="-1456636592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,7 +1489,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404661696"/>
+        <c:crossAx val="-1456633328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1584,11 +1730,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404656256"/>
-        <c:axId val="404666592"/>
+        <c:axId val="-1456639856"/>
+        <c:axId val="-1456635504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404656256"/>
+        <c:axId val="-1456639856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,12 +1786,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404666592"/>
+        <c:crossAx val="-1456635504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404666592"/>
+        <c:axId val="-1456635504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +1847,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404656256"/>
+        <c:crossAx val="-1456639856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1792,7 +1938,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1964,11 +2109,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404659520"/>
-        <c:axId val="404657344"/>
+        <c:axId val="-1456803776"/>
+        <c:axId val="-1456799968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404659520"/>
+        <c:axId val="-1456803776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,12 +2165,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404657344"/>
+        <c:crossAx val="-1456799968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404657344"/>
+        <c:axId val="-1456799968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2226,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404659520"/>
+        <c:crossAx val="-1456803776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2148,7 +2293,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2323,11 +2467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404670400"/>
-        <c:axId val="404660064"/>
+        <c:axId val="-1456803232"/>
+        <c:axId val="-1456802688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404670400"/>
+        <c:axId val="-1456803232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2379,12 +2523,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404660064"/>
+        <c:crossAx val="-1456802688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404660064"/>
+        <c:axId val="-1456802688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2440,7 +2584,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404670400"/>
+        <c:crossAx val="-1456803232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2507,7 +2651,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2682,11 +2825,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404661152"/>
-        <c:axId val="404663872"/>
+        <c:axId val="-1456798880"/>
+        <c:axId val="-1456802144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404661152"/>
+        <c:axId val="-1456798880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,12 +2881,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404663872"/>
+        <c:crossAx val="-1456802144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404663872"/>
+        <c:axId val="-1456802144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2799,7 +2942,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404661152"/>
+        <c:crossAx val="-1456798880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2866,7 +3009,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3041,11 +3183,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="404665504"/>
-        <c:axId val="404668224"/>
+        <c:axId val="-1408495632"/>
+        <c:axId val="-1408498352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="404665504"/>
+        <c:axId val="-1408495632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,12 +3239,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404668224"/>
+        <c:crossAx val="-1408498352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="404668224"/>
+        <c:axId val="-1408498352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3158,7 +3300,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="404665504"/>
+        <c:crossAx val="-1408495632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8302,22 +8444,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="H3" s="11" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -8609,6 +8751,525 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="18">
+        <v>140</v>
+      </c>
+      <c r="C4" s="3">
+        <v>135</v>
+      </c>
+      <c r="D4" s="3">
+        <v>483</v>
+      </c>
+      <c r="E4" s="3">
+        <v>615</v>
+      </c>
+      <c r="F4" s="3">
+        <v>139</v>
+      </c>
+      <c r="G4" s="3">
+        <v>72</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6318</v>
+      </c>
+      <c r="I4" s="3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
+      <c r="B5" s="18">
+        <v>163</v>
+      </c>
+      <c r="C5" s="3">
+        <v>131</v>
+      </c>
+      <c r="D5" s="3">
+        <v>472</v>
+      </c>
+      <c r="E5" s="3">
+        <v>651</v>
+      </c>
+      <c r="F5" s="3">
+        <v>131</v>
+      </c>
+      <c r="G5" s="3">
+        <v>67</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6317</v>
+      </c>
+      <c r="I5" s="3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="18">
+        <v>149</v>
+      </c>
+      <c r="C6" s="3">
+        <v>129</v>
+      </c>
+      <c r="D6" s="3">
+        <v>507</v>
+      </c>
+      <c r="E6" s="3">
+        <v>626</v>
+      </c>
+      <c r="F6" s="3">
+        <v>202</v>
+      </c>
+      <c r="G6" s="3">
+        <v>42</v>
+      </c>
+      <c r="H6" s="3">
+        <v>6329</v>
+      </c>
+      <c r="I6" s="3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="18">
+        <v>135</v>
+      </c>
+      <c r="C7" s="3">
+        <v>134</v>
+      </c>
+      <c r="D7" s="3">
+        <v>510</v>
+      </c>
+      <c r="E7" s="3">
+        <v>614</v>
+      </c>
+      <c r="F7" s="3">
+        <v>177</v>
+      </c>
+      <c r="G7" s="3">
+        <v>45</v>
+      </c>
+      <c r="H7" s="3">
+        <v>6321</v>
+      </c>
+      <c r="I7" s="3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="18">
+        <v>149</v>
+      </c>
+      <c r="C8" s="3">
+        <v>134</v>
+      </c>
+      <c r="D8" s="3">
+        <v>459</v>
+      </c>
+      <c r="E8" s="3">
+        <v>683</v>
+      </c>
+      <c r="F8" s="3">
+        <v>140</v>
+      </c>
+      <c r="G8" s="3">
+        <v>60</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6316</v>
+      </c>
+      <c r="I8" s="3">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="18">
+        <v>140</v>
+      </c>
+      <c r="C9" s="3">
+        <v>151</v>
+      </c>
+      <c r="D9" s="3">
+        <v>492</v>
+      </c>
+      <c r="E9" s="3">
+        <v>642</v>
+      </c>
+      <c r="F9" s="3">
+        <v>145</v>
+      </c>
+      <c r="G9" s="3">
+        <v>65</v>
+      </c>
+      <c r="H9" s="3">
+        <v>6335</v>
+      </c>
+      <c r="I9" s="3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="18">
+        <v>134</v>
+      </c>
+      <c r="C10" s="3">
+        <v>154</v>
+      </c>
+      <c r="D10" s="3">
+        <v>507</v>
+      </c>
+      <c r="E10" s="3">
+        <v>655</v>
+      </c>
+      <c r="F10" s="3">
+        <v>188</v>
+      </c>
+      <c r="G10" s="3">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6338</v>
+      </c>
+      <c r="I10" s="3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="18">
+        <v>183</v>
+      </c>
+      <c r="C11" s="3">
+        <v>164</v>
+      </c>
+      <c r="D11" s="3">
+        <v>439</v>
+      </c>
+      <c r="E11" s="3">
+        <v>654</v>
+      </c>
+      <c r="F11" s="3">
+        <v>179</v>
+      </c>
+      <c r="G11" s="3">
+        <v>48</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6330</v>
+      </c>
+      <c r="I11" s="3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="18">
+        <v>171</v>
+      </c>
+      <c r="C12" s="3">
+        <v>141</v>
+      </c>
+      <c r="D12" s="3">
+        <v>427</v>
+      </c>
+      <c r="E12" s="3">
+        <v>649</v>
+      </c>
+      <c r="F12" s="3">
+        <v>176</v>
+      </c>
+      <c r="G12" s="3">
+        <v>57</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6327</v>
+      </c>
+      <c r="I12" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
+      <c r="B13" s="18">
+        <v>180</v>
+      </c>
+      <c r="C13" s="3">
+        <v>170</v>
+      </c>
+      <c r="D13" s="3">
+        <v>476</v>
+      </c>
+      <c r="E13" s="3">
+        <v>610</v>
+      </c>
+      <c r="F13" s="3">
+        <v>151</v>
+      </c>
+      <c r="G13" s="3">
+        <v>66</v>
+      </c>
+      <c r="H13" s="3">
+        <v>6326</v>
+      </c>
+      <c r="I13" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="18">
+        <v>139</v>
+      </c>
+      <c r="C14" s="3">
+        <v>134</v>
+      </c>
+      <c r="D14" s="3">
+        <v>486</v>
+      </c>
+      <c r="E14" s="3">
+        <v>661</v>
+      </c>
+      <c r="F14" s="3">
+        <v>165</v>
+      </c>
+      <c r="G14" s="3">
+        <v>79</v>
+      </c>
+      <c r="H14" s="3">
+        <v>6320</v>
+      </c>
+      <c r="I14" s="3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="19">
+        <f>(B4+B5+B6+B7+B8+B9+B10+B11+B12+B13+B14)/11</f>
+        <v>153</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" ref="C16:I16" si="0">(C4+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14)/11</f>
+        <v>143.36363636363637</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>641.81818181818187</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>60.18181818181818</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>6325.181818181818</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>304.81818181818181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>MAX(B4:B14)</f>
+        <v>183</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:I17" si="1">MAX(C4:C14)</f>
+        <v>170</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="1"/>
+        <v>510</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>683</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="1"/>
+        <v>202</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>6338</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2">
+        <f>MIN(B4:B14)</f>
+        <v>134</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:I18" si="2">MIN(C4:C14)</f>
+        <v>129</v>
+      </c>
+      <c r="D18" s="26">
+        <f t="shared" si="2"/>
+        <v>427</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="2"/>
+        <v>610</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="2"/>
+        <v>6316</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <f>D18</f>
+        <v>427</v>
+      </c>
+      <c r="C21">
+        <f>I17</f>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>1100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="A2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:G27"/>
   <sheetViews>
@@ -8862,11 +9523,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
@@ -8884,12 +9545,12 @@
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="5" t="s">
         <v>7</v>
       </c>
@@ -9029,12 +9690,12 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="5" t="s">
         <v>7</v>
       </c>
@@ -9175,12 +9836,12 @@
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="5" t="s">
         <v>7</v>
       </c>
@@ -9330,12 +9991,12 @@
       <c r="B30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
       <c r="G30" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>